<commit_message>
Updated code to latest changes
</commit_message>
<xml_diff>
--- a/Resource/Credential.xlsx
+++ b/Resource/Credential.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chirag\owls\OWLS_Automation\OWLS_Automation\Resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Genix\OWLS\Workspace\com.genix.owls.automation\OWLS_Automation\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="6855"/>
   </bookViews>
   <sheets>
     <sheet name="Potal" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="CRM-Inspection" sheetId="3" r:id="rId3"/>
     <sheet name="CRM_Delegates" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>URL</t>
   </si>
@@ -51,9 +51,6 @@
     <t>IOAuto</t>
   </si>
   <si>
-    <t>DOAuto</t>
-  </si>
-  <si>
     <t>CRM User- Inspection</t>
   </si>
   <si>
@@ -63,10 +60,10 @@
     <t>admin</t>
   </si>
   <si>
-    <t>chirag.kiwiqa</t>
-  </si>
-  <si>
-    <t>chirag!</t>
+    <t>ankit.patel</t>
+  </si>
+  <si>
+    <t>patel12!</t>
   </si>
 </sst>
 </file>
@@ -527,7 +524,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -563,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +580,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +614,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,7 +643,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +654,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -768,7 +765,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -802,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>